<commit_message>
Added LandP Ryegrass simulation
</commit_message>
<xml_diff>
--- a/Tests/Validation/Ryegrass/Gatton9597.xlsx
+++ b/Tests/Validation/Ryegrass/Gatton9597.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jessica\GIT\ApsimX\ApsimX\Tests\Validation\Ryegrass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3392AEB-DF3F-4A18-A942-949CF96CDD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEA91F8-F561-4F46-8A80-2EBD274B6FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-3975" windowWidth="38640" windowHeight="21120" xr2:uid="{F6FAA82E-3A16-4146-BEFE-CA22E4777305}"/>
+    <workbookView xWindow="44565" yWindow="795" windowWidth="28800" windowHeight="15150" xr2:uid="{F6FAA82E-3A16-4146-BEFE-CA22E4777305}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CBB69E-72C1-4422-8074-459BD3868199}">
   <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -455,20 +458,20 @@
     <col min="5" max="5" width="29.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>